<commit_message>
Mise à jour des types d'erreurs .xlsx , ajout des bulles Gauche/droite, mise à jour du .gitignore
</commit_message>
<xml_diff>
--- a/Sources/types_err.xlsx
+++ b/Sources/types_err.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milio\PycharmProjects\Stage\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6555AC-0C31-4CED-88E5-120D222C5552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D64CB4-EBE4-42B4-8BD9-435316856118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Types</t>
   </si>
@@ -31,86 +31,92 @@
     <t>Materiel</t>
   </si>
   <si>
-    <t>Planification</t>
-  </si>
-  <si>
-    <t>Mauvaise interpretation</t>
-  </si>
-  <si>
-    <t>Reflexe</t>
-  </si>
-  <si>
-    <t>Intérruption</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
-    <t>Interférence intéraction</t>
-  </si>
-  <si>
     <t>Oubli</t>
   </si>
   <si>
     <t>Prévention</t>
   </si>
   <si>
-    <t>Blue Screen, Freeze</t>
-  </si>
-  <si>
     <t>Exemple</t>
   </si>
   <si>
-    <t>Incident négatif de pointage / Missclick : Faute User/Système</t>
-  </si>
-  <si>
-    <t>Incident négatif matériel</t>
-  </si>
-  <si>
-    <t>Cliquer à côté d'un bouton (mal viser/Bug vous empêchant de bien cliquer)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oubli de faire quelque chose </t>
-  </si>
-  <si>
-    <t>Oublier de joindre la pièce jointe</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Ne pas enregistrer ses données sur un disque dur, perdre ses données à cause de cela</t>
-  </si>
-  <si>
-    <t>Notification apparaissant sous le doigt au moment d'appuyer, entraînant un clic accidentel.</t>
-  </si>
-  <si>
-    <t>Notification imprévue interrompant une tâche en cours.????</t>
-  </si>
-  <si>
-    <t>Réflexe d'annuler ou de confirmer une action par habitude.</t>
-  </si>
-  <si>
-    <t>Fermeture par réflexe de la pop-up 'Le saviez-vous' sur une application, ce qui empêche de lire l'information intéressante affichée.</t>
-  </si>
-  <si>
-    <t>Mauvaise communication entre l'utilisateur et le système</t>
-  </si>
-  <si>
-    <t>Interaction involontaire et inévitable</t>
-  </si>
-  <si>
-    <t>Perte de concentration en raison d'une interruption soudaine</t>
-  </si>
-  <si>
-    <t>Ne pas faire quelque chose que l'on devrait faire qui causera potentiellement un problème à longterme</t>
+    <t>Le système ralentit au point de devenir pénible à utiliser, ou cesse complètement de réagir.</t>
+  </si>
+  <si>
+    <t>Problème de connexion bluetooth, problèmes de câblage, de périphérique, de connexion, de batterie, de surchauffe</t>
+  </si>
+  <si>
+    <t>Interprétation par l'utilisateur</t>
+  </si>
+  <si>
+    <t>L’interprétation que vous faites de l’effet d’une commande ou d’une action est erronée.</t>
+  </si>
+  <si>
+    <t>Icône pas claire ou pas assez visible, textes trop longs ou pas assez vulgarisés, îcones ou raccourcis qui sortent des standards</t>
+  </si>
+  <si>
+    <t>Interprétation par le système</t>
+  </si>
+  <si>
+    <t>Le système interprète vos actions, vos commandes ou vos gestes de la mauvaise manière.</t>
+  </si>
+  <si>
+    <t>L'assistant vocal s'active par erreur, erreur d'autocorrect, erreur de traduction, erreur de GPS</t>
+  </si>
+  <si>
+    <t>Perturbation</t>
+  </si>
+  <si>
+    <t>Perturbation cognitive au cours d’une tâche. Vous êtes déconcentré par un événement de l’interface, vous avez oublié ce que vous étiez en train de faire.</t>
+  </si>
+  <si>
+    <t>Réception d'un mail/message/notification pendant une activité de concentration</t>
+  </si>
+  <si>
+    <t>Interférence d'interaction</t>
+  </si>
+  <si>
+    <t>Faute de frappe, scroll au mauvais endroit de la page, erreur de visée dans un jeu</t>
+  </si>
+  <si>
+    <t>Mauvais réflexe</t>
+  </si>
+  <si>
+    <t>Utiliser une action habituelle dans un contexte où elle ne s'applique pas, voire peut produire des effets non désirés.</t>
+  </si>
+  <si>
+    <t>Utilisation du mauvais raccourci, habitude de disposition des icônes qui mène à des erreurs de clics lors d'un changement, fermer trop vite ses notifications</t>
+  </si>
+  <si>
+    <t>Oubli ou remise au lendemain d’une action de prévention, un “au cas-où”</t>
+  </si>
+  <si>
+    <t>Ne pas faire une mise à jour jusqu'au dernier moment possible, ne pas faire de sauvegarde séparée</t>
+  </si>
+  <si>
+    <t>Oubli d’une étape dans l’exécution d’une tâche, d’une séquence d’actions.</t>
+  </si>
+  <si>
+    <t>Oublier la pièce jointe d'un mail, oublier d'enregistrer avant de compiler ou push sur un git, oublier de changer de calque avant de modifier un dessin</t>
+  </si>
+  <si>
+    <t>Cliquer ou "taper" à côté de l'objet visé : un bouton, un lien, un email, une cible, une touche de clavier etc. \n Le clic peut soit se produire "dans le vide" (sans conséquence), soit activer un autre objet ou fenêtre non visé(e).</t>
+  </si>
+  <si>
+    <t>L'interface change juste avant un clic ou l'appui sur une touche : une pop-up apparait, une liste se met à jour, une autre application \n prend le focus, etc. Cela a pour conséquence que ce clic se produit "dans le vide" ou sur un objet non désiré. </t>
+  </si>
+  <si>
+    <t>Mise à jour de la liste d'autocomplétion pendant l'entrée d'un texte, on sélectionne l'élément qui vient tout juste de changer sans \n pouvoir réagir. Clic "capturé" au dernier moment par une popup ou une notification. Boîte de dialogue ou raccourcis disparaît juste avant le clic.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +128,18 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,11 +177,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,15 +488,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.86328125" customWidth="1"/>
-    <col min="2" max="2" width="50.53125" customWidth="1"/>
-    <col min="3" max="3" width="99.86328125" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="209.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="236.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -487,109 +507,110 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reste à faire : changement de tableau bad toujours '' ?, stimulation. Fait : changement du comportement de changement de tableau et de display des tableaux
</commit_message>
<xml_diff>
--- a/Sources/types_err.xlsx
+++ b/Sources/types_err.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milio\PycharmProjects\Stage\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D64CB4-EBE4-42B4-8BD9-435316856118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC69C7A-7C67-486B-92CA-52EE572FF0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>L’interprétation que vous faites de l’effet d’une commande ou d’une action est erronée.</t>
   </si>
   <si>
-    <t>Icône pas claire ou pas assez visible, textes trop longs ou pas assez vulgarisés, îcones ou raccourcis qui sortent des standards</t>
-  </si>
-  <si>
     <t>Interprétation par le système</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>Perturbation</t>
   </si>
   <si>
-    <t>Perturbation cognitive au cours d’une tâche. Vous êtes déconcentré par un événement de l’interface, vous avez oublié ce que vous étiez en train de faire.</t>
-  </si>
-  <si>
     <t>Réception d'un mail/message/notification pendant une activité de concentration</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>Utiliser une action habituelle dans un contexte où elle ne s'applique pas, voire peut produire des effets non désirés.</t>
   </si>
   <si>
-    <t>Utilisation du mauvais raccourci, habitude de disposition des icônes qui mène à des erreurs de clics lors d'un changement, fermer trop vite ses notifications</t>
-  </si>
-  <si>
     <t>Oubli ou remise au lendemain d’une action de prévention, un “au cas-où”</t>
   </si>
   <si>
@@ -100,9 +91,6 @@
     <t>Oubli d’une étape dans l’exécution d’une tâche, d’une séquence d’actions.</t>
   </si>
   <si>
-    <t>Oublier la pièce jointe d'un mail, oublier d'enregistrer avant de compiler ou push sur un git, oublier de changer de calque avant de modifier un dessin</t>
-  </si>
-  <si>
     <t>Cliquer ou "taper" à côté de l'objet visé : un bouton, un lien, un email, une cible, une touche de clavier etc. \n Le clic peut soit se produire "dans le vide" (sans conséquence), soit activer un autre objet ou fenêtre non visé(e).</t>
   </si>
   <si>
@@ -110,6 +98,18 @@
   </si>
   <si>
     <t>Mise à jour de la liste d'autocomplétion pendant l'entrée d'un texte, on sélectionne l'élément qui vient tout juste de changer sans \n pouvoir réagir. Clic "capturé" au dernier moment par une popup ou une notification. Boîte de dialogue ou raccourcis disparaît juste avant le clic.</t>
+  </si>
+  <si>
+    <t>Oublier la pièce jointe d'un mail, oublier d'enregistrer avant de compiler ou push sur un git, \n oublier de changer de calque avant de modifier un dessin</t>
+  </si>
+  <si>
+    <t>Utilisation du mauvais raccourci, habitude de disposition des icônes qui mène à des erreurs de clics lors d'un changement, \n fermer trop vite ses notifications</t>
+  </si>
+  <si>
+    <t>Perturbation cognitive au cours d’une tâche. Vous êtes déconcentré par un événement de l’interface, \n vous avez oublié ce que vous étiez en train de faire.</t>
+  </si>
+  <si>
+    <t>Icône pas claire ou pas assez visible, textes trop longs ou pas assez vulgarisés,  \n îcones ou raccourcis qui sortent des standards</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -529,29 +529,29 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -559,10 +559,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -570,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -578,13 +578,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -592,21 +592,21 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>